<commit_message>
Added Caacitor values and removed bad columns from BOM
</commit_message>
<xml_diff>
--- a/poweramp/Power Amp BOM.xlsx
+++ b/poweramp/Power Amp BOM.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="44">
   <si>
     <t>Comment</t>
   </si>
@@ -28,12 +28,6 @@
     <t>Digikey No</t>
   </si>
   <si>
-    <t>Digikey No.</t>
-  </si>
-  <si>
-    <t>Digikey Number</t>
-  </si>
-  <si>
     <t>Footprint</t>
   </si>
   <si>
@@ -149,6 +143,9 @@
   </si>
   <si>
     <t>535-11573-1-ND for L1 and 535-11563-6-ND for L2</t>
+  </si>
+  <si>
+    <t>C1, C2: 399-8106-1-ND, C3: 490-6441-1-ND , C4, C5, C6, C7: 490-8295-1-ND, C8: 490-6441-1-ND, C8: 399-11171-1-ND, C9: 445-5978-1-ND, C11: 445-5978-1-ND , C12: 399-8106-1-ND, C13:399-11166-1-ND, C14: 399-9239-1-ND, C15: 490-6441-1-ND, C16:399-3129-1-ND  C17: 445-5978-1-ND</t>
   </si>
 </sst>
 </file>
@@ -217,8 +214,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -526,300 +524,255 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="E1" sqref="E1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="3" width="10.85546875" customWidth="1"/>
     <col min="4" max="4" width="33.85546875" customWidth="1"/>
-    <col min="5" max="10" width="10.85546875" customWidth="1"/>
+    <col min="5" max="8" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="D2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="4">
+        <v>17</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="E3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H2" s="2" t="s">
+      <c r="G3" s="4">
+        <v>3</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="3">
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="B4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3" s="3">
+      <c r="G4" s="4">
         <v>3</v>
       </c>
-      <c r="J3" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="2" t="s">
+      <c r="H4" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="2" t="s">
+      <c r="B5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I4" s="3">
+      <c r="D5" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="4">
+        <v>2</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="4">
+        <v>1</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" s="4">
         <v>3</v>
       </c>
-      <c r="J4" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="H7" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B8" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I5" s="3">
-        <v>2</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I6" s="3">
+      <c r="F8" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G8" s="4">
+        <v>3</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G9" s="4">
         <v>1</v>
       </c>
-      <c r="J6" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="I7" s="3">
-        <v>3</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="I8" s="3">
-        <v>3</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="I9" s="3">
-        <v>1</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D13" s="4"/>
+      <c r="H9" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D13" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>